<commit_message>
Split directions into Setup and Play
</commit_message>
<xml_diff>
--- a/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
+++ b/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\MeadInflowSimulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192E92E8-97BC-4411-BE61-B32F6E01BF45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC544CF-93F2-434E-BC40-F03D25B84EC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8950" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
   </bookViews>
@@ -383,9 +383,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -393,6 +390,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E479131-29BE-4E82-B456-BDEC50237677}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,7 +866,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="22" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="str">
+      <c r="A11" s="26" t="str">
         <f>LowerBasinCuts!$A$4</f>
         <v>Mead Elev (ft)</v>
       </c>
@@ -925,15 +925,15 @@
         <f>LowerBasinCuts!B5</f>
         <v>5.981122</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="27">
         <f>LowerBasinCuts!I5/1000</f>
         <v>0.72</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <f>LowerBasinCuts!J5/1000</f>
         <v>0.03</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="27">
         <f>LowerBasinCuts!K5/1000</f>
         <v>0.35</v>
       </c>
@@ -941,7 +941,7 @@
         <f>LowerBasinCuts!O5</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <f>SUM(C12:F12)</f>
         <v>1.375</v>
       </c>
@@ -954,23 +954,23 @@
         <v>5.981122</v>
       </c>
       <c r="K12" s="25">
-        <f>(K$9-C12)/($O$9-SUM($C12:$F12))</f>
+        <f t="shared" ref="K12:O19" si="2">(K$9-C12)/($O$9-SUM($C12:$F12))</f>
         <v>0.27278688524590167</v>
       </c>
       <c r="L12" s="25">
-        <f>(L$9-D12)/($O$9-SUM($C12:$F12))</f>
+        <f t="shared" si="2"/>
         <v>3.5409836065573776E-2</v>
       </c>
       <c r="M12" s="25">
-        <f>(M$9-E12)/($O$9-SUM($C12:$F12))</f>
+        <f t="shared" si="2"/>
         <v>0.53114754098360661</v>
       </c>
       <c r="N12" s="25">
-        <f>(N$9-F12)/($O$9-SUM($C12:$F12))</f>
+        <f t="shared" si="2"/>
         <v>0.16065573770491803</v>
       </c>
       <c r="O12" s="25">
-        <f>(O$9-G12)/($O$9-SUM($C12:$F12))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -983,15 +983,15 @@
         <f>LowerBasinCuts!B6</f>
         <v>6.305377</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="27">
         <f>LowerBasinCuts!I6/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <f>LowerBasinCuts!J6/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="27">
         <f>LowerBasinCuts!K6/1000</f>
         <v>0.35</v>
       </c>
@@ -999,36 +999,36 @@
         <f>LowerBasinCuts!O6</f>
         <v>0.17100000000000001</v>
       </c>
-      <c r="G13" s="28">
-        <f t="shared" ref="G13:G14" si="2">SUM(C13:F13)</f>
+      <c r="G13" s="27">
+        <f t="shared" ref="G13:G14" si="3">SUM(C13:F13)</f>
         <v>1.1879999999999999</v>
       </c>
       <c r="I13" s="24">
-        <f t="shared" ref="I13:I19" si="3">A13</f>
+        <f t="shared" ref="I13:I19" si="4">A13</f>
         <v>1030</v>
       </c>
       <c r="J13" s="11">
-        <f t="shared" ref="J13:J19" si="4">B13</f>
+        <f t="shared" ref="J13:J19" si="5">B13</f>
         <v>6.305377</v>
       </c>
       <c r="K13" s="25">
-        <f>(K$9-C13)/($O$9-SUM($C13:$F13))</f>
+        <f t="shared" si="2"/>
         <v>0.27649769585253453</v>
       </c>
       <c r="L13" s="25">
-        <f>(L$9-D13)/($O$9-SUM($C13:$F13))</f>
+        <f t="shared" si="2"/>
         <v>3.4946236559139782E-2</v>
       </c>
       <c r="M13" s="25">
-        <f>(M$9-E13)/($O$9-SUM($C13:$F13))</f>
+        <f t="shared" si="2"/>
         <v>0.51843317972350234</v>
       </c>
       <c r="N13" s="25">
-        <f>(N$9-F13)/($O$9-SUM($C13:$F13))</f>
+        <f t="shared" si="2"/>
         <v>0.17012288786482332</v>
       </c>
       <c r="O13" s="25">
-        <f>(O$9-G13)/($O$9-SUM($C13:$F13))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1041,15 +1041,15 @@
         <f>LowerBasinCuts!B7</f>
         <v>6.6375080000000004</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="27">
         <f>LowerBasinCuts!I7/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="27">
         <f>LowerBasinCuts!J7/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="27">
         <f>LowerBasinCuts!K7/1000</f>
         <v>0.3</v>
       </c>
@@ -1057,36 +1057,36 @@
         <f>LowerBasinCuts!O7</f>
         <v>0.16200000000000001</v>
       </c>
-      <c r="G14" s="28">
-        <f t="shared" si="2"/>
+      <c r="G14" s="27">
+        <f t="shared" si="3"/>
         <v>1.129</v>
       </c>
       <c r="I14" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1035</v>
       </c>
       <c r="J14" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.6375080000000004</v>
       </c>
       <c r="K14" s="25">
-        <f>(K$9-C14)/($O$9-SUM($C14:$F14))</f>
+        <f t="shared" si="2"/>
         <v>0.27442510481514415</v>
       </c>
       <c r="L14" s="25">
-        <f>(L$9-D14)/($O$9-SUM($C14:$F14))</f>
+        <f t="shared" si="2"/>
         <v>3.4684284080802943E-2</v>
       </c>
       <c r="M14" s="25">
-        <f>(M$9-E14)/($O$9-SUM($C14:$F14))</f>
+        <f t="shared" si="2"/>
         <v>0.52089950451022748</v>
       </c>
       <c r="N14" s="25">
-        <f>(N$9-F14)/($O$9-SUM($C14:$F14))</f>
+        <f t="shared" si="2"/>
         <v>0.16999110659382544</v>
       </c>
       <c r="O14" s="25">
-        <f>(O$9-G14)/($O$9-SUM($C14:$F14))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1099,15 +1099,15 @@
         <f>LowerBasinCuts!B8</f>
         <v>6.977665</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="27">
         <f>LowerBasinCuts!I8/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="27">
         <f>LowerBasinCuts!J8/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="27">
         <f>LowerBasinCuts!K8/1000</f>
         <v>0.25</v>
       </c>
@@ -1115,36 +1115,36 @@
         <f>LowerBasinCuts!O8</f>
         <v>0.154</v>
       </c>
-      <c r="G15" s="28">
-        <f t="shared" ref="G15:G19" si="5">SUM(C15:F15)</f>
+      <c r="G15" s="27">
+        <f t="shared" ref="G15:G19" si="6">SUM(C15:F15)</f>
         <v>1.071</v>
       </c>
       <c r="I15" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1040</v>
       </c>
       <c r="J15" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.977665</v>
       </c>
       <c r="K15" s="25">
-        <f>(K$9-C15)/($O$9-SUM($C15:$F15))</f>
+        <f t="shared" si="2"/>
         <v>0.27241770715096475</v>
       </c>
       <c r="L15" s="25">
-        <f>(L$9-D15)/($O$9-SUM($C15:$F15))</f>
+        <f t="shared" si="2"/>
         <v>3.4430571320469158E-2</v>
       </c>
       <c r="M15" s="25">
-        <f>(M$9-E15)/($O$9-SUM($C15:$F15))</f>
+        <f t="shared" si="2"/>
         <v>0.52339513179467778</v>
       </c>
       <c r="N15" s="25">
-        <f>(N$9-F15)/($O$9-SUM($C15:$F15))</f>
+        <f t="shared" si="2"/>
         <v>0.16975658973388827</v>
       </c>
       <c r="O15" s="25">
-        <f>(O$9-G15)/($O$9-SUM($C15:$F15))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1157,15 +1157,15 @@
         <f>LowerBasinCuts!B9</f>
         <v>7.3260519999999998</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="27">
         <f>LowerBasinCuts!I9/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="27">
         <f>LowerBasinCuts!J9/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="27">
         <f>LowerBasinCuts!K9/1000</f>
         <v>0.2</v>
       </c>
@@ -1173,36 +1173,36 @@
         <f>LowerBasinCuts!O9</f>
         <v>0.14599999999999999</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="27">
+        <f t="shared" si="6"/>
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="I16" s="24">
+        <f t="shared" si="4"/>
+        <v>1045</v>
+      </c>
+      <c r="J16" s="11">
         <f t="shared" si="5"/>
-        <v>1.0129999999999999</v>
-      </c>
-      <c r="I16" s="24">
-        <f t="shared" si="3"/>
-        <v>1045</v>
-      </c>
-      <c r="J16" s="11">
-        <f t="shared" si="4"/>
         <v>7.3260519999999998</v>
       </c>
       <c r="K16" s="25">
-        <f>(K$9-C16)/($O$9-SUM($C16:$F16))</f>
+        <f t="shared" si="2"/>
         <v>0.27043946412920994</v>
       </c>
       <c r="L16" s="25">
-        <f>(L$9-D16)/($O$9-SUM($C16:$F16))</f>
+        <f t="shared" si="2"/>
         <v>3.4180543382997364E-2</v>
       </c>
       <c r="M16" s="25">
-        <f>(M$9-E16)/($O$9-SUM($C16:$F16))</f>
+        <f t="shared" si="2"/>
         <v>0.52585451358457491</v>
       </c>
       <c r="N16" s="25">
-        <f>(N$9-F16)/($O$9-SUM($C16:$F16))</f>
+        <f t="shared" si="2"/>
         <v>0.16952547890321773</v>
       </c>
       <c r="O16" s="25">
-        <f>(O$9-G16)/($O$9-SUM($C16:$F16))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1215,15 +1215,15 @@
         <f>LowerBasinCuts!B10</f>
         <v>7.6828779999999997</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="27">
         <f>LowerBasinCuts!I10/1000</f>
         <v>0.59199999999999997</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <f>LowerBasinCuts!J10/1000</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="27">
         <f>LowerBasinCuts!K10/1000</f>
         <v>0</v>
       </c>
@@ -1231,36 +1231,36 @@
         <f>LowerBasinCuts!O10</f>
         <v>0.104</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="27">
+        <f t="shared" si="6"/>
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="I17" s="24">
+        <f t="shared" si="4"/>
+        <v>1050</v>
+      </c>
+      <c r="J17" s="11">
         <f t="shared" si="5"/>
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="I17" s="24">
-        <f t="shared" si="3"/>
-        <v>1050</v>
-      </c>
-      <c r="J17" s="11">
-        <f t="shared" si="4"/>
         <v>7.6828779999999997</v>
       </c>
       <c r="K17" s="25">
-        <f>(K$9-C17)/($O$9-SUM($C17:$F17))</f>
+        <f t="shared" si="2"/>
         <v>0.26669887667592701</v>
       </c>
       <c r="L17" s="25">
-        <f>(L$9-D17)/($O$9-SUM($C17:$F17))</f>
+        <f t="shared" si="2"/>
         <v>3.3216572049764463E-2</v>
       </c>
       <c r="M17" s="25">
-        <f>(M$9-E17)/($O$9-SUM($C17:$F17))</f>
+        <f t="shared" si="2"/>
         <v>0.53146515279623152</v>
       </c>
       <c r="N17" s="25">
-        <f>(N$9-F17)/($O$9-SUM($C17:$F17))</f>
+        <f t="shared" si="2"/>
         <v>0.16861939847807705</v>
       </c>
       <c r="O17" s="25">
-        <f>(O$9-G17)/($O$9-SUM($C17:$F17))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1273,15 +1273,15 @@
         <f>LowerBasinCuts!B11</f>
         <v>9.6009879999900001</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="27">
         <f>LowerBasinCuts!I11/1000</f>
         <v>0.51200000000000001</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="27">
         <f>LowerBasinCuts!J11/1000</f>
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="27">
         <f>LowerBasinCuts!K11/1000</f>
         <v>0</v>
       </c>
@@ -1289,36 +1289,36 @@
         <f>LowerBasinCuts!O11</f>
         <v>0.08</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="27">
+        <f t="shared" si="6"/>
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="I18" s="24">
+        <f t="shared" si="4"/>
+        <v>1075</v>
+      </c>
+      <c r="J18" s="11">
         <f t="shared" si="5"/>
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="I18" s="24">
-        <f t="shared" si="3"/>
-        <v>1075</v>
-      </c>
-      <c r="J18" s="11">
-        <f t="shared" si="4"/>
         <v>9.6009879999900001</v>
       </c>
       <c r="K18" s="25">
-        <f>(K$9-C18)/($O$9-SUM($C18:$F18))</f>
+        <f t="shared" si="2"/>
         <v>0.27280314772862763</v>
       </c>
       <c r="L18" s="25">
-        <f>(L$9-D18)/($O$9-SUM($C18:$F18))</f>
+        <f t="shared" si="2"/>
         <v>3.3265768451174432E-2</v>
       </c>
       <c r="M18" s="25">
-        <f>(M$9-E18)/($O$9-SUM($C18:$F18))</f>
+        <f t="shared" si="2"/>
         <v>0.52462143793966853</v>
       </c>
       <c r="N18" s="25">
-        <f>(N$9-F18)/($O$9-SUM($C18:$F18))</f>
+        <f t="shared" si="2"/>
         <v>0.16930964588052938</v>
       </c>
       <c r="O18" s="25">
-        <f>(O$9-G18)/($O$9-SUM($C18:$F18))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1331,15 +1331,15 @@
         <f>LowerBasinCuts!B12</f>
         <v>10.857008</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="27">
         <f>LowerBasinCuts!I12/1000</f>
         <v>0.192</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="27">
         <f>LowerBasinCuts!J12/1000</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="27">
         <f>LowerBasinCuts!K12/1000</f>
         <v>0</v>
       </c>
@@ -1347,36 +1347,36 @@
         <f>LowerBasinCuts!O12</f>
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="27">
+        <f t="shared" si="6"/>
+        <v>0.24100000000000002</v>
+      </c>
+      <c r="I19" s="24">
+        <f t="shared" si="4"/>
+        <v>1090</v>
+      </c>
+      <c r="J19" s="11">
         <f t="shared" si="5"/>
-        <v>0.24100000000000002</v>
-      </c>
-      <c r="I19" s="24">
-        <f t="shared" si="3"/>
-        <v>1090</v>
-      </c>
-      <c r="J19" s="11">
-        <f t="shared" si="4"/>
         <v>10.857008</v>
       </c>
       <c r="K19" s="25">
-        <f>(K$9-C19)/($O$9-SUM($C19:$F19))</f>
+        <f t="shared" si="2"/>
         <v>0.29775088480420137</v>
       </c>
       <c r="L19" s="25">
-        <f>(L$9-D19)/($O$9-SUM($C19:$F19))</f>
+        <f t="shared" si="2"/>
         <v>3.3337138942801686E-2</v>
       </c>
       <c r="M19" s="25">
-        <f>(M$9-E19)/($O$9-SUM($C19:$F19))</f>
+        <f t="shared" si="2"/>
         <v>0.50234044982303916</v>
       </c>
       <c r="N19" s="25">
-        <f>(N$9-F19)/($O$9-SUM($C19:$F19))</f>
+        <f t="shared" si="2"/>
         <v>0.16657152642995776</v>
       </c>
       <c r="O19" s="25">
-        <f>(O$9-G19)/($O$9-SUM($C19:$F19))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>1045</v>
+        <v>1030</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
@@ -1459,15 +1459,15 @@
       </c>
       <c r="E27" s="7">
         <f>VLOOKUP($A$23,$A$12:$G$19,COLUMN(E25)-COLUMN($A$25)+1)</f>
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="F27" s="7">
         <f>VLOOKUP($A$23,$A$12:$G$19,COLUMN(F25)-COLUMN($A$25)+1)</f>
-        <v>0.14599999999999999</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="G27" s="7">
         <f>VLOOKUP($A$23,$A$12:$G$19,COLUMN(G25)-COLUMN($A$25)+1)</f>
-        <v>1.0129999999999999</v>
+        <v>1.1879999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -1479,20 +1479,20 @@
         <v>2.1599999999999997</v>
       </c>
       <c r="D28" s="7">
-        <f t="shared" ref="D28:G28" si="6">D26-D27</f>
+        <f t="shared" ref="D28:G28" si="7">D26-D27</f>
         <v>0.27299999999999996</v>
       </c>
       <c r="E28" s="7">
-        <f t="shared" si="6"/>
-        <v>4.2</v>
+        <f t="shared" si="7"/>
+        <v>4.0500000000000007</v>
       </c>
       <c r="F28" s="7">
-        <f t="shared" si="6"/>
-        <v>1.3540000000000001</v>
+        <f t="shared" si="7"/>
+        <v>1.329</v>
       </c>
       <c r="G28" s="7">
-        <f t="shared" si="6"/>
-        <v>7.9870000000000001</v>
+        <f t="shared" si="7"/>
+        <v>7.8120000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
@@ -1501,22 +1501,22 @@
       </c>
       <c r="C29" s="20">
         <f>C28/$G$28</f>
-        <v>0.27043946412920994</v>
+        <v>0.27649769585253453</v>
       </c>
       <c r="D29" s="20">
-        <f t="shared" ref="D29:G29" si="7">D28/$G$28</f>
-        <v>3.4180543382997364E-2</v>
+        <f t="shared" ref="D29:G29" si="8">D28/$G$28</f>
+        <v>3.4946236559139782E-2</v>
       </c>
       <c r="E29" s="20">
-        <f t="shared" si="7"/>
-        <v>0.52585451358457491</v>
+        <f t="shared" si="8"/>
+        <v>0.51843317972350234</v>
       </c>
       <c r="F29" s="20">
-        <f t="shared" si="7"/>
-        <v>0.16952547890321773</v>
+        <f t="shared" si="8"/>
+        <v>0.17012288786482332</v>
       </c>
       <c r="G29" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -1526,7 +1526,7 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1572,25 +1572,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="M3" s="26" t="s">
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="M3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">

</xml_diff>

<commit_message>
Update Mead simulations to include 1,060 feet
</commit_message>
<xml_diff>
--- a/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
+++ b/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\MeadInflowSimulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC544CF-93F2-434E-BC40-F03D25B84EC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEB2F49-BA1F-4FD9-B2CC-A7926BFAB544}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8950" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8950" activeTab="1" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="ShareOfInflow" sheetId="2" r:id="rId1"/>
-    <sheet name="LowerBasinCuts" sheetId="1" r:id="rId2"/>
+    <sheet name="ShareOfInflowByElevation" sheetId="2" r:id="rId1"/>
+    <sheet name="ShareOfInflowByInflowVolume" sheetId="3" r:id="rId2"/>
+    <sheet name="LowerBasinCuts" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Mandatory Cutbacks according to 2007 Interim Guidelines, 2019 Drought Contingency Plan, and Minutes 319 and 323</t>
   </si>
@@ -127,9 +128,6 @@
     <t>Lower Basin Shares</t>
   </si>
   <si>
-    <t>Calculate each Lower Basin Party's and Mexico's share of Lake Mead inflow</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Mandatory Conservation Target (maf/year) </t>
     </r>
@@ -189,6 +187,27 @@
   </si>
   <si>
     <t>Requested Citation:</t>
+  </si>
+  <si>
+    <t>Calculate each Lower Basin Party's and Mexico's share of Lake Mead inflow by Reservoir Elevation</t>
+  </si>
+  <si>
+    <t>Share of Inflow by Inflow Volume</t>
+  </si>
+  <si>
+    <t>A. Principle of Equality</t>
+  </si>
+  <si>
+    <t>Annual Inflow (maf)</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>Lifeline</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -312,7 +331,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -393,6 +412,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -411,6 +436,1378 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ShareOfInflowByInflowVolume!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$14:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16065573770491803</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32131147540983607</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4819672131147541</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64262295081967213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80327868852459017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9639344262295082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1245901639344262</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2852459016393443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4459016393442623</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6065573770491803</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E60F-4874-9203-43D64D988F45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ShareOfInflowByInflowVolume!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>California</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$13:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53114754098360661</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0622950819672132</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5934426229508198</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1245901639344265</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6557377049180331</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1868852459016397</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7180327868852463</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.2491803278688529</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.78032786885246</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.3114754098360661</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E60F-4874-9203-43D64D988F45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ShareOfInflowByInflowVolume!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nevada</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$12:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5409836065573776E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0819672131147551E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10622950819672133</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1416393442622951</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17704918032786887</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.21245901639344267</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24786885245901644</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28327868852459021</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.318688524590164</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35409836065573774</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E60F-4874-9203-43D64D988F45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ShareOfInflowByInflowVolume!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Arizona</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ShareOfInflowByInflowVolume!$C$11:$M$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27278688524590167</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54557377049180333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.818360655737705</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0911475409836067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3639344262295083</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.63672131147541</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9095081967213117</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1822950819672133</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4550819672131148</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7278688524590167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E60F-4874-9203-43D64D988F45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1711104096"/>
+        <c:axId val="821636576"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="1711104096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Lake Mead Inflow</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>(maf per year)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44199467764721345"/>
+              <c:y val="0.74897055209139307"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="821636576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="821636576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Share of Inflow</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>(maf</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> per year)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1711104096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,6 +1881,47 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>408517</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>78846</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>105833</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>126471</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7654CC0C-1607-4995-9C32-FF4A7946316C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -788,8 +2226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E479131-29BE-4E82-B456-BDEC50237677}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,7 +2245,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -818,7 +2256,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -828,7 +2266,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -859,7 +2297,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>32</v>
@@ -1522,12 +2960,12 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1540,6 +2978,585 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4760DCDC-D4B4-460D-B53A-F996DA439874}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18:N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C9" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>6</v>
+      </c>
+      <c r="J10" s="2">
+        <v>7</v>
+      </c>
+      <c r="K10" s="2">
+        <v>8</v>
+      </c>
+      <c r="L10" s="2">
+        <v>9</v>
+      </c>
+      <c r="M10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="30">
+        <f>ShareOfInflowByElevation!$K$12</f>
+        <v>0.27278688524590167</v>
+      </c>
+      <c r="C11" s="7">
+        <f>$B11*C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" ref="D11:M14" si="0">$B11*D$10</f>
+        <v>0.27278688524590167</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.54557377049180333</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0911475409836067</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3639344262295083</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.63672131147541</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="0"/>
+        <v>1.9095081967213117</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.1822950819672133</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4550819672131148</v>
+      </c>
+      <c r="M11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.7278688524590167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="30">
+        <f>ShareOfInflowByElevation!$L$12</f>
+        <v>3.5409836065573776E-2</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" ref="C12:C14" si="1">$B12*C$10</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>3.5409836065573776E-2</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>7.0819672131147551E-2</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.10622950819672133</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.1416393442622951</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.17704918032786887</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.21245901639344267</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.24786885245901644</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.28327868852459021</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.318688524590164</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.35409836065573774</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="30">
+        <f>ShareOfInflowByElevation!$M$12</f>
+        <v>0.53114754098360661</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.53114754098360661</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0622950819672132</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="0"/>
+        <v>1.5934426229508198</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>2.1245901639344265</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="0"/>
+        <v>2.6557377049180331</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>3.1868852459016397</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="0"/>
+        <v>3.7180327868852463</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="0"/>
+        <v>4.2491803278688529</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="0"/>
+        <v>4.78032786885246</v>
+      </c>
+      <c r="M13" s="7">
+        <f t="shared" si="0"/>
+        <v>5.3114754098360661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="30">
+        <f>ShareOfInflowByElevation!$N$12</f>
+        <v>0.16065573770491803</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.16065573770491803</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.32131147540983607</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.4819672131147541</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.64262295081967213</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.80327868852459017</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9639344262295082</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.1245901639344262</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2852459016393443</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4459016393442623</v>
+      </c>
+      <c r="M14" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6065573770491803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3</v>
+      </c>
+      <c r="H17" s="2">
+        <v>4</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5</v>
+      </c>
+      <c r="J17" s="2">
+        <v>6</v>
+      </c>
+      <c r="K17" s="2">
+        <v>7</v>
+      </c>
+      <c r="L17" s="2">
+        <v>8</v>
+      </c>
+      <c r="M17" s="2">
+        <v>9</v>
+      </c>
+      <c r="N17" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="30">
+        <f>ShareOfInflowByElevation!$K$12</f>
+        <v>0.27278688524590167</v>
+      </c>
+      <c r="C18" s="2">
+        <f>ShareOfInflowByElevation!K9-ShareOfInflowByElevation!C12</f>
+        <v>2.08</v>
+      </c>
+      <c r="D18" s="7">
+        <f>$B18*C$10</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <f>$B18*D$10</f>
+        <v>0.27278688524590167</v>
+      </c>
+      <c r="F18" s="7">
+        <f>$B18*E$10</f>
+        <v>0.54557377049180333</v>
+      </c>
+      <c r="G18" s="7">
+        <f>$B18*F$10</f>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="H18" s="7">
+        <f>IF(H19&lt;$C19,G18,G18+H$17-SUM(G16:G18,H19))</f>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="I18" s="7">
+        <f>IF(I19&lt;$C19,H18,H18+I$17-SUM(H16:H18,I19))</f>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" ref="J18:N18" si="2">IF(J19&lt;$C19,I18,I18+J$17-SUM(I16:I18,J19))</f>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="2"/>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="2"/>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="M18" s="7">
+        <f t="shared" si="2"/>
+        <v>0.818360655737705</v>
+      </c>
+      <c r="N18" s="7">
+        <f t="shared" si="2"/>
+        <v>0.818360655737705</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="30">
+        <f>ShareOfInflowByElevation!$L$12</f>
+        <v>3.5409836065573776E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <f>ShareOfInflowByElevation!L9-ShareOfInflowByElevation!D12</f>
+        <v>0.27</v>
+      </c>
+      <c r="D19" s="7">
+        <f>$B19*C$10</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <f>$B19*D$10</f>
+        <v>3.5409836065573776E-2</v>
+      </c>
+      <c r="F19" s="7">
+        <f>$B19*E$10</f>
+        <v>7.0819672131147551E-2</v>
+      </c>
+      <c r="G19" s="7">
+        <f>$B19*F$10</f>
+        <v>0.10622950819672133</v>
+      </c>
+      <c r="H19" s="7">
+        <f>IF(H20&lt;$C20,G19,G19+H$17-SUM(G17:G19,H20))</f>
+        <v>0.10622950819672133</v>
+      </c>
+      <c r="I19" s="7">
+        <f>IF(I20&lt;$C20,H19,H19+I$17-SUM(H17:H19,I20))</f>
+        <v>0.10622950819672133</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" ref="J19:N19" si="3">IF(J20&lt;$C20,I19,I19+J$17-SUM(I17:I19,J20))</f>
+        <v>0.10622950819672133</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="3"/>
+        <v>-4.6687704918032775</v>
+      </c>
+      <c r="L19" s="7">
+        <f t="shared" si="3"/>
+        <v>-10.443770491803276</v>
+      </c>
+      <c r="M19" s="7">
+        <f t="shared" si="3"/>
+        <v>-17.218770491803276</v>
+      </c>
+      <c r="N19" s="7">
+        <f t="shared" si="3"/>
+        <v>-24.993770491803275</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="30">
+        <f>ShareOfInflowByElevation!$M$12</f>
+        <v>0.53114754098360661</v>
+      </c>
+      <c r="C20" s="2">
+        <f>ShareOfInflowByElevation!M9-ShareOfInflowByElevation!E12</f>
+        <v>4.0500000000000007</v>
+      </c>
+      <c r="D20" s="7">
+        <f>$B20*C$10</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <f>$B20*D$10</f>
+        <v>0.53114754098360661</v>
+      </c>
+      <c r="F20" s="7">
+        <f>$B20*E$10</f>
+        <v>1.0622950819672132</v>
+      </c>
+      <c r="G20" s="7">
+        <f>$B20*F$10</f>
+        <v>1.5934426229508198</v>
+      </c>
+      <c r="H20" s="7">
+        <f>IF(H21&lt;$C21,G20,G20+H$17-SUM(G18:G20,H21))</f>
+        <v>1.8504098360655732</v>
+      </c>
+      <c r="I20" s="7">
+        <f>IF(I21&lt;$C21,H20,H20+I$17-SUM(H18:H20,I21))</f>
+        <v>2.8504098360655736</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" ref="J20:N20" si="4">IF(J21&lt;$C21,I20,I20+J$17-SUM(I18:I20,J21))</f>
+        <v>3.8504098360655732</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="4"/>
+        <v>4.8504098360655732</v>
+      </c>
+      <c r="L20" s="7">
+        <f t="shared" si="4"/>
+        <v>10.625409836065572</v>
+      </c>
+      <c r="M20" s="7">
+        <f t="shared" si="4"/>
+        <v>17.40040983606557</v>
+      </c>
+      <c r="N20" s="7">
+        <f t="shared" si="4"/>
+        <v>25.175409836065569</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="30">
+        <f>ShareOfInflowByElevation!$N$12</f>
+        <v>0.16065573770491803</v>
+      </c>
+      <c r="C21" s="2">
+        <f>ShareOfInflowByElevation!N9-ShareOfInflowByElevation!F12</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D21" s="7">
+        <f>$B21*C$10</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <f>$B21*D$10</f>
+        <v>0.16065573770491803</v>
+      </c>
+      <c r="F21" s="7">
+        <f>$B21*E$10</f>
+        <v>0.32131147540983607</v>
+      </c>
+      <c r="G21" s="7">
+        <f>$B21*F$10</f>
+        <v>0.4819672131147541</v>
+      </c>
+      <c r="H21" s="7">
+        <f>IF(G21&gt;=$C21,$C21,MIN(G21+H17-G17,$C21))</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="I21" s="7">
+        <f>IF(H21&gt;=$C21,$C21,MIN(H21+I17-H17,$C21))</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" ref="J21:N21" si="5">IF(I21&gt;=$C21,$C21,MIN(I21+J17-I17,$C21))</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="5"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="L21" s="7">
+        <f t="shared" si="5"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="M21" s="7">
+        <f t="shared" si="5"/>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="N21" s="7">
+        <f t="shared" si="5"/>
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H22" s="7">
+        <f>SUM(H18:H21)</f>
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="I22" s="7">
+        <f>SUM(I18:I21)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C9:M9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C23DD7-389E-4635-B2D0-E8AC525AFF63}">
   <dimension ref="A1:P36"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update share of inflow workbooks
</commit_message>
<xml_diff>
--- a/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
+++ b/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\MeadInflowSimulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEB2F49-BA1F-4FD9-B2CC-A7926BFAB544}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71F6884-16AE-4547-985B-B0B3024DA9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8950" activeTab="1" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8950" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
   </bookViews>
   <sheets>
     <sheet name="ShareOfInflowByElevation" sheetId="2" r:id="rId1"/>
-    <sheet name="ShareOfInflowByInflowVolume" sheetId="3" r:id="rId2"/>
-    <sheet name="LowerBasinCuts" sheetId="1" r:id="rId3"/>
+    <sheet name="LowerBasinCuts" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Mandatory Cutbacks according to 2007 Interim Guidelines, 2019 Drought Contingency Plan, and Minutes 319 and 323</t>
   </si>
@@ -190,24 +189,6 @@
   </si>
   <si>
     <t>Calculate each Lower Basin Party's and Mexico's share of Lake Mead inflow by Reservoir Elevation</t>
-  </si>
-  <si>
-    <t>Share of Inflow by Inflow Volume</t>
-  </si>
-  <si>
-    <t>A. Principle of Equality</t>
-  </si>
-  <si>
-    <t>Annual Inflow (maf)</t>
-  </si>
-  <si>
-    <t>Party</t>
-  </si>
-  <si>
-    <t>Lifeline</t>
-  </si>
-  <si>
-    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -331,7 +312,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -412,12 +393,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -436,1378 +411,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ShareOfInflowByInflowVolume!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mexico</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$14:$M$14</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16065573770491803</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.32131147540983607</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.4819672131147541</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.64262295081967213</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.80327868852459017</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.9639344262295082</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1245901639344262</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.2852459016393443</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.4459016393442623</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.6065573770491803</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E60F-4874-9203-43D64D988F45}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ShareOfInflowByInflowVolume!$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>California</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$13:$M$13</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.53114754098360661</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0622950819672132</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5934426229508198</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.1245901639344265</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6557377049180331</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.1868852459016397</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.7180327868852463</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.2491803278688529</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.78032786885246</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.3114754098360661</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E60F-4874-9203-43D64D988F45}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ShareOfInflowByInflowVolume!$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Nevada</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$12:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.5409836065573776E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.0819672131147551E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.10622950819672133</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1416393442622951</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.17704918032786887</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.21245901639344267</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.24786885245901644</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.28327868852459021</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.318688524590164</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.35409836065573774</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E60F-4874-9203-43D64D988F45}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ShareOfInflowByInflowVolume!$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Arizona</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="20000"/>
-                <a:lumOff val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:cat>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$10:$M$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ShareOfInflowByInflowVolume!$C$11:$M$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27278688524590167</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.54557377049180333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.818360655737705</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0911475409836067</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3639344262295083</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.63672131147541</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.9095081967213117</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.1822950819672133</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.4550819672131148</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.7278688524590167</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E60F-4874-9203-43D64D988F45}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1711104096"/>
-        <c:axId val="821636576"/>
-      </c:areaChart>
-      <c:catAx>
-        <c:axId val="1711104096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Lake Mead Inflow</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="1"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>(maf per year)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.44199467764721345"/>
-              <c:y val="0.74897055209139307"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="821636576"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="821636576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>Share of Inflow</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="1"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" b="1"/>
-                  <a:t>(maf</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" b="1" baseline="0"/>
-                  <a:t> per year)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" b="1"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1711104096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1881,47 +484,6 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>408517</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>78846</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>105833</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>126471</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7654CC0C-1607-4995-9C32-FF4A7946316C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2226,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E479131-29BE-4E82-B456-BDEC50237677}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="K11" sqref="K11:N11"/>
     </sheetView>
   </sheetViews>
@@ -2978,585 +1540,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4760DCDC-D4B4-460D-B53A-F996DA439874}">
-  <dimension ref="A1:N22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18:N21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C9" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2">
-        <v>3</v>
-      </c>
-      <c r="G10" s="2">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2">
-        <v>5</v>
-      </c>
-      <c r="I10" s="2">
-        <v>6</v>
-      </c>
-      <c r="J10" s="2">
-        <v>7</v>
-      </c>
-      <c r="K10" s="2">
-        <v>8</v>
-      </c>
-      <c r="L10" s="2">
-        <v>9</v>
-      </c>
-      <c r="M10" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="30">
-        <f>ShareOfInflowByElevation!$K$12</f>
-        <v>0.27278688524590167</v>
-      </c>
-      <c r="C11" s="7">
-        <f>$B11*C$10</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <f t="shared" ref="D11:M14" si="0">$B11*D$10</f>
-        <v>0.27278688524590167</v>
-      </c>
-      <c r="E11" s="7">
-        <f t="shared" si="0"/>
-        <v>0.54557377049180333</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="0"/>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="0"/>
-        <v>1.0911475409836067</v>
-      </c>
-      <c r="H11" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3639344262295083</v>
-      </c>
-      <c r="I11" s="7">
-        <f t="shared" si="0"/>
-        <v>1.63672131147541</v>
-      </c>
-      <c r="J11" s="7">
-        <f t="shared" si="0"/>
-        <v>1.9095081967213117</v>
-      </c>
-      <c r="K11" s="7">
-        <f t="shared" si="0"/>
-        <v>2.1822950819672133</v>
-      </c>
-      <c r="L11" s="7">
-        <f t="shared" si="0"/>
-        <v>2.4550819672131148</v>
-      </c>
-      <c r="M11" s="7">
-        <f t="shared" si="0"/>
-        <v>2.7278688524590167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="30">
-        <f>ShareOfInflowByElevation!$L$12</f>
-        <v>3.5409836065573776E-2</v>
-      </c>
-      <c r="C12" s="7">
-        <f t="shared" ref="C12:C14" si="1">$B12*C$10</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="7">
-        <f t="shared" si="0"/>
-        <v>3.5409836065573776E-2</v>
-      </c>
-      <c r="E12" s="7">
-        <f t="shared" si="0"/>
-        <v>7.0819672131147551E-2</v>
-      </c>
-      <c r="F12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.10622950819672133</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.1416393442622951</v>
-      </c>
-      <c r="H12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.17704918032786887</v>
-      </c>
-      <c r="I12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.21245901639344267</v>
-      </c>
-      <c r="J12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.24786885245901644</v>
-      </c>
-      <c r="K12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.28327868852459021</v>
-      </c>
-      <c r="L12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.318688524590164</v>
-      </c>
-      <c r="M12" s="7">
-        <f t="shared" si="0"/>
-        <v>0.35409836065573774</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="30">
-        <f>ShareOfInflowByElevation!$M$12</f>
-        <v>0.53114754098360661</v>
-      </c>
-      <c r="C13" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.53114754098360661</v>
-      </c>
-      <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>1.0622950819672132</v>
-      </c>
-      <c r="F13" s="7">
-        <f t="shared" si="0"/>
-        <v>1.5934426229508198</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="0"/>
-        <v>2.1245901639344265</v>
-      </c>
-      <c r="H13" s="7">
-        <f t="shared" si="0"/>
-        <v>2.6557377049180331</v>
-      </c>
-      <c r="I13" s="7">
-        <f t="shared" si="0"/>
-        <v>3.1868852459016397</v>
-      </c>
-      <c r="J13" s="7">
-        <f t="shared" si="0"/>
-        <v>3.7180327868852463</v>
-      </c>
-      <c r="K13" s="7">
-        <f t="shared" si="0"/>
-        <v>4.2491803278688529</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" si="0"/>
-        <v>4.78032786885246</v>
-      </c>
-      <c r="M13" s="7">
-        <f t="shared" si="0"/>
-        <v>5.3114754098360661</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="30">
-        <f>ShareOfInflowByElevation!$N$12</f>
-        <v>0.16065573770491803</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="7">
-        <f t="shared" si="0"/>
-        <v>0.16065573770491803</v>
-      </c>
-      <c r="E14" s="7">
-        <f t="shared" si="0"/>
-        <v>0.32131147540983607</v>
-      </c>
-      <c r="F14" s="7">
-        <f t="shared" si="0"/>
-        <v>0.4819672131147541</v>
-      </c>
-      <c r="G14" s="7">
-        <f t="shared" si="0"/>
-        <v>0.64262295081967213</v>
-      </c>
-      <c r="H14" s="7">
-        <f t="shared" si="0"/>
-        <v>0.80327868852459017</v>
-      </c>
-      <c r="I14" s="7">
-        <f t="shared" si="0"/>
-        <v>0.9639344262295082</v>
-      </c>
-      <c r="J14" s="7">
-        <f t="shared" si="0"/>
-        <v>1.1245901639344262</v>
-      </c>
-      <c r="K14" s="7">
-        <f t="shared" si="0"/>
-        <v>1.2852459016393443</v>
-      </c>
-      <c r="L14" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4459016393442623</v>
-      </c>
-      <c r="M14" s="7">
-        <f t="shared" si="0"/>
-        <v>1.6065573770491803</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <v>2</v>
-      </c>
-      <c r="G17" s="2">
-        <v>3</v>
-      </c>
-      <c r="H17" s="2">
-        <v>4</v>
-      </c>
-      <c r="I17" s="2">
-        <v>5</v>
-      </c>
-      <c r="J17" s="2">
-        <v>6</v>
-      </c>
-      <c r="K17" s="2">
-        <v>7</v>
-      </c>
-      <c r="L17" s="2">
-        <v>8</v>
-      </c>
-      <c r="M17" s="2">
-        <v>9</v>
-      </c>
-      <c r="N17" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="30">
-        <f>ShareOfInflowByElevation!$K$12</f>
-        <v>0.27278688524590167</v>
-      </c>
-      <c r="C18" s="2">
-        <f>ShareOfInflowByElevation!K9-ShareOfInflowByElevation!C12</f>
-        <v>2.08</v>
-      </c>
-      <c r="D18" s="7">
-        <f>$B18*C$10</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="7">
-        <f>$B18*D$10</f>
-        <v>0.27278688524590167</v>
-      </c>
-      <c r="F18" s="7">
-        <f>$B18*E$10</f>
-        <v>0.54557377049180333</v>
-      </c>
-      <c r="G18" s="7">
-        <f>$B18*F$10</f>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="H18" s="7">
-        <f>IF(H19&lt;$C19,G18,G18+H$17-SUM(G16:G18,H19))</f>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="I18" s="7">
-        <f>IF(I19&lt;$C19,H18,H18+I$17-SUM(H16:H18,I19))</f>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="J18" s="7">
-        <f t="shared" ref="J18:N18" si="2">IF(J19&lt;$C19,I18,I18+J$17-SUM(I16:I18,J19))</f>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="K18" s="7">
-        <f t="shared" si="2"/>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="L18" s="7">
-        <f t="shared" si="2"/>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="M18" s="7">
-        <f t="shared" si="2"/>
-        <v>0.818360655737705</v>
-      </c>
-      <c r="N18" s="7">
-        <f t="shared" si="2"/>
-        <v>0.818360655737705</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="30">
-        <f>ShareOfInflowByElevation!$L$12</f>
-        <v>3.5409836065573776E-2</v>
-      </c>
-      <c r="C19" s="2">
-        <f>ShareOfInflowByElevation!L9-ShareOfInflowByElevation!D12</f>
-        <v>0.27</v>
-      </c>
-      <c r="D19" s="7">
-        <f>$B19*C$10</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
-        <f>$B19*D$10</f>
-        <v>3.5409836065573776E-2</v>
-      </c>
-      <c r="F19" s="7">
-        <f>$B19*E$10</f>
-        <v>7.0819672131147551E-2</v>
-      </c>
-      <c r="G19" s="7">
-        <f>$B19*F$10</f>
-        <v>0.10622950819672133</v>
-      </c>
-      <c r="H19" s="7">
-        <f>IF(H20&lt;$C20,G19,G19+H$17-SUM(G17:G19,H20))</f>
-        <v>0.10622950819672133</v>
-      </c>
-      <c r="I19" s="7">
-        <f>IF(I20&lt;$C20,H19,H19+I$17-SUM(H17:H19,I20))</f>
-        <v>0.10622950819672133</v>
-      </c>
-      <c r="J19" s="7">
-        <f t="shared" ref="J19:N19" si="3">IF(J20&lt;$C20,I19,I19+J$17-SUM(I17:I19,J20))</f>
-        <v>0.10622950819672133</v>
-      </c>
-      <c r="K19" s="7">
-        <f t="shared" si="3"/>
-        <v>-4.6687704918032775</v>
-      </c>
-      <c r="L19" s="7">
-        <f t="shared" si="3"/>
-        <v>-10.443770491803276</v>
-      </c>
-      <c r="M19" s="7">
-        <f t="shared" si="3"/>
-        <v>-17.218770491803276</v>
-      </c>
-      <c r="N19" s="7">
-        <f t="shared" si="3"/>
-        <v>-24.993770491803275</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="30">
-        <f>ShareOfInflowByElevation!$M$12</f>
-        <v>0.53114754098360661</v>
-      </c>
-      <c r="C20" s="2">
-        <f>ShareOfInflowByElevation!M9-ShareOfInflowByElevation!E12</f>
-        <v>4.0500000000000007</v>
-      </c>
-      <c r="D20" s="7">
-        <f>$B20*C$10</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <f>$B20*D$10</f>
-        <v>0.53114754098360661</v>
-      </c>
-      <c r="F20" s="7">
-        <f>$B20*E$10</f>
-        <v>1.0622950819672132</v>
-      </c>
-      <c r="G20" s="7">
-        <f>$B20*F$10</f>
-        <v>1.5934426229508198</v>
-      </c>
-      <c r="H20" s="7">
-        <f>IF(H21&lt;$C21,G20,G20+H$17-SUM(G18:G20,H21))</f>
-        <v>1.8504098360655732</v>
-      </c>
-      <c r="I20" s="7">
-        <f>IF(I21&lt;$C21,H20,H20+I$17-SUM(H18:H20,I21))</f>
-        <v>2.8504098360655736</v>
-      </c>
-      <c r="J20" s="7">
-        <f t="shared" ref="J20:N20" si="4">IF(J21&lt;$C21,I20,I20+J$17-SUM(I18:I20,J21))</f>
-        <v>3.8504098360655732</v>
-      </c>
-      <c r="K20" s="7">
-        <f t="shared" si="4"/>
-        <v>4.8504098360655732</v>
-      </c>
-      <c r="L20" s="7">
-        <f t="shared" si="4"/>
-        <v>10.625409836065572</v>
-      </c>
-      <c r="M20" s="7">
-        <f t="shared" si="4"/>
-        <v>17.40040983606557</v>
-      </c>
-      <c r="N20" s="7">
-        <f t="shared" si="4"/>
-        <v>25.175409836065569</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="30">
-        <f>ShareOfInflowByElevation!$N$12</f>
-        <v>0.16065573770491803</v>
-      </c>
-      <c r="C21" s="2">
-        <f>ShareOfInflowByElevation!N9-ShareOfInflowByElevation!F12</f>
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="D21" s="7">
-        <f>$B21*C$10</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <f>$B21*D$10</f>
-        <v>0.16065573770491803</v>
-      </c>
-      <c r="F21" s="7">
-        <f>$B21*E$10</f>
-        <v>0.32131147540983607</v>
-      </c>
-      <c r="G21" s="7">
-        <f>$B21*F$10</f>
-        <v>0.4819672131147541</v>
-      </c>
-      <c r="H21" s="7">
-        <f>IF(G21&gt;=$C21,$C21,MIN(G21+H17-G17,$C21))</f>
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="I21" s="7">
-        <f>IF(H21&gt;=$C21,$C21,MIN(H21+I17-H17,$C21))</f>
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="J21" s="7">
-        <f t="shared" ref="J21:N21" si="5">IF(I21&gt;=$C21,$C21,MIN(I21+J17-I17,$C21))</f>
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="K21" s="7">
-        <f t="shared" si="5"/>
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="L21" s="7">
-        <f t="shared" si="5"/>
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="M21" s="7">
-        <f t="shared" si="5"/>
-        <v>1.2250000000000001</v>
-      </c>
-      <c r="N21" s="7">
-        <f t="shared" si="5"/>
-        <v>1.2250000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="H22" s="7">
-        <f>SUM(H18:H21)</f>
-        <v>3.9999999999999996</v>
-      </c>
-      <c r="I22" s="7">
-        <f>SUM(I18:I21)</f>
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C9:M9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C23DD7-389E-4635-B2D0-E8AC525AFF63}">
   <dimension ref="A1:P36"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update text in Protect Lake Powell to get to readable form
</commit_message>
<xml_diff>
--- a/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
+++ b/MeadInflowSimulations/ShareOfInflow-LB-MX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\MeadInflowSimulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71F6884-16AE-4547-985B-B0B3024DA9CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800E2205-A190-4B09-BD69-9EA3C186FD62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8950" xr2:uid="{B7E24150-B936-4491-85FE-E2B15A6311EA}"/>
   </bookViews>
@@ -312,7 +312,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -374,17 +374,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,6 +386,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -789,7 +786,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:N11"/>
+      <selection activeCell="I11" sqref="I11:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,7 +863,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="22" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="str">
+      <c r="A11" s="3" t="str">
         <f>LowerBasinCuts!$A$4</f>
         <v>Mead Elev (ft)</v>
       </c>
@@ -889,29 +886,29 @@
       <c r="G11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="23" t="str">
+      <c r="K11" s="28" t="str">
         <f t="shared" ref="K11:M11" si="0">C11</f>
         <v>Arizona</v>
       </c>
-      <c r="L11" s="23" t="str">
+      <c r="L11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>Nevada</v>
       </c>
-      <c r="M11" s="23" t="str">
+      <c r="M11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>California</v>
       </c>
-      <c r="N11" s="23" t="str">
+      <c r="N11" s="28" t="str">
         <f>F11</f>
         <v>Mexico</v>
       </c>
-      <c r="O11" s="23" t="str">
+      <c r="O11" s="28" t="str">
         <f t="shared" ref="O11" si="1">G11</f>
         <v>Total</v>
       </c>
@@ -925,15 +922,15 @@
         <f>LowerBasinCuts!B5</f>
         <v>5.981122</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="25">
         <f>LowerBasinCuts!I5/1000</f>
         <v>0.72</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="25">
         <f>LowerBasinCuts!J5/1000</f>
         <v>0.03</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="25">
         <f>LowerBasinCuts!K5/1000</f>
         <v>0.35</v>
       </c>
@@ -941,11 +938,11 @@
         <f>LowerBasinCuts!O5</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="25">
         <f>SUM(C12:F12)</f>
         <v>1.375</v>
       </c>
-      <c r="I12" s="24">
+      <c r="I12" s="23">
         <f>A12</f>
         <v>1025</v>
       </c>
@@ -953,23 +950,23 @@
         <f>B12</f>
         <v>5.981122</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="24">
         <f t="shared" ref="K12:O19" si="2">(K$9-C12)/($O$9-SUM($C12:$F12))</f>
         <v>0.27278688524590167</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="24">
         <f t="shared" si="2"/>
         <v>3.5409836065573776E-2</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="24">
         <f t="shared" si="2"/>
         <v>0.53114754098360661</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="24">
         <f t="shared" si="2"/>
         <v>0.16065573770491803</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -983,15 +980,15 @@
         <f>LowerBasinCuts!B6</f>
         <v>6.305377</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="25">
         <f>LowerBasinCuts!I6/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="25">
         <f>LowerBasinCuts!J6/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="25">
         <f>LowerBasinCuts!K6/1000</f>
         <v>0.35</v>
       </c>
@@ -999,11 +996,11 @@
         <f>LowerBasinCuts!O6</f>
         <v>0.17100000000000001</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="25">
         <f t="shared" ref="G13:G14" si="3">SUM(C13:F13)</f>
         <v>1.1879999999999999</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="23">
         <f t="shared" ref="I13:I19" si="4">A13</f>
         <v>1030</v>
       </c>
@@ -1011,23 +1008,23 @@
         <f t="shared" ref="J13:J19" si="5">B13</f>
         <v>6.305377</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="24">
         <f t="shared" si="2"/>
         <v>0.27649769585253453</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="24">
         <f t="shared" si="2"/>
         <v>3.4946236559139782E-2</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="24">
         <f t="shared" si="2"/>
         <v>0.51843317972350234</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="24">
         <f t="shared" si="2"/>
         <v>0.17012288786482332</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1041,15 +1038,15 @@
         <f>LowerBasinCuts!B7</f>
         <v>6.6375080000000004</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="25">
         <f>LowerBasinCuts!I7/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="25">
         <f>LowerBasinCuts!J7/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="25">
         <f>LowerBasinCuts!K7/1000</f>
         <v>0.3</v>
       </c>
@@ -1057,11 +1054,11 @@
         <f>LowerBasinCuts!O7</f>
         <v>0.16200000000000001</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="25">
         <f t="shared" si="3"/>
         <v>1.129</v>
       </c>
-      <c r="I14" s="24">
+      <c r="I14" s="23">
         <f t="shared" si="4"/>
         <v>1035</v>
       </c>
@@ -1069,23 +1066,23 @@
         <f t="shared" si="5"/>
         <v>6.6375080000000004</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="24">
         <f t="shared" si="2"/>
         <v>0.27442510481514415</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="24">
         <f t="shared" si="2"/>
         <v>3.4684284080802943E-2</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="24">
         <f t="shared" si="2"/>
         <v>0.52089950451022748</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="24">
         <f t="shared" si="2"/>
         <v>0.16999110659382544</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1099,15 +1096,15 @@
         <f>LowerBasinCuts!B8</f>
         <v>6.977665</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="25">
         <f>LowerBasinCuts!I8/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="25">
         <f>LowerBasinCuts!J8/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="25">
         <f>LowerBasinCuts!K8/1000</f>
         <v>0.25</v>
       </c>
@@ -1115,11 +1112,11 @@
         <f>LowerBasinCuts!O8</f>
         <v>0.154</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="25">
         <f t="shared" ref="G15:G19" si="6">SUM(C15:F15)</f>
         <v>1.071</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="23">
         <f t="shared" si="4"/>
         <v>1040</v>
       </c>
@@ -1127,23 +1124,23 @@
         <f t="shared" si="5"/>
         <v>6.977665</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="24">
         <f t="shared" si="2"/>
         <v>0.27241770715096475</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="24">
         <f t="shared" si="2"/>
         <v>3.4430571320469158E-2</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="24">
         <f t="shared" si="2"/>
         <v>0.52339513179467778</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="24">
         <f t="shared" si="2"/>
         <v>0.16975658973388827</v>
       </c>
-      <c r="O15" s="25">
+      <c r="O15" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1157,15 +1154,15 @@
         <f>LowerBasinCuts!B9</f>
         <v>7.3260519999999998</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="25">
         <f>LowerBasinCuts!I9/1000</f>
         <v>0.64</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="25">
         <f>LowerBasinCuts!J9/1000</f>
         <v>2.7E-2</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="25">
         <f>LowerBasinCuts!K9/1000</f>
         <v>0.2</v>
       </c>
@@ -1173,11 +1170,11 @@
         <f>LowerBasinCuts!O9</f>
         <v>0.14599999999999999</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="25">
         <f t="shared" si="6"/>
         <v>1.0129999999999999</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16" s="23">
         <f t="shared" si="4"/>
         <v>1045</v>
       </c>
@@ -1185,23 +1182,23 @@
         <f t="shared" si="5"/>
         <v>7.3260519999999998</v>
       </c>
-      <c r="K16" s="25">
+      <c r="K16" s="24">
         <f t="shared" si="2"/>
         <v>0.27043946412920994</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="24">
         <f t="shared" si="2"/>
         <v>3.4180543382997364E-2</v>
       </c>
-      <c r="M16" s="25">
+      <c r="M16" s="24">
         <f t="shared" si="2"/>
         <v>0.52585451358457491</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="24">
         <f t="shared" si="2"/>
         <v>0.16952547890321773</v>
       </c>
-      <c r="O16" s="25">
+      <c r="O16" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1215,15 +1212,15 @@
         <f>LowerBasinCuts!B10</f>
         <v>7.6828779999999997</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="25">
         <f>LowerBasinCuts!I10/1000</f>
         <v>0.59199999999999997</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="25">
         <f>LowerBasinCuts!J10/1000</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="25">
         <f>LowerBasinCuts!K10/1000</f>
         <v>0</v>
       </c>
@@ -1231,11 +1228,11 @@
         <f>LowerBasinCuts!O10</f>
         <v>0.104</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="25">
         <f t="shared" si="6"/>
         <v>0.72099999999999997</v>
       </c>
-      <c r="I17" s="24">
+      <c r="I17" s="23">
         <f t="shared" si="4"/>
         <v>1050</v>
       </c>
@@ -1243,23 +1240,23 @@
         <f t="shared" si="5"/>
         <v>7.6828779999999997</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="24">
         <f t="shared" si="2"/>
         <v>0.26669887667592701</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="24">
         <f t="shared" si="2"/>
         <v>3.3216572049764463E-2</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="24">
         <f t="shared" si="2"/>
         <v>0.53146515279623152</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="24">
         <f t="shared" si="2"/>
         <v>0.16861939847807705</v>
       </c>
-      <c r="O17" s="25">
+      <c r="O17" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1273,15 +1270,15 @@
         <f>LowerBasinCuts!B11</f>
         <v>9.6009879999900001</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="25">
         <f>LowerBasinCuts!I11/1000</f>
         <v>0.51200000000000001</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="25">
         <f>LowerBasinCuts!J11/1000</f>
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="25">
         <f>LowerBasinCuts!K11/1000</f>
         <v>0</v>
       </c>
@@ -1289,11 +1286,11 @@
         <f>LowerBasinCuts!O11</f>
         <v>0.08</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="25">
         <f t="shared" si="6"/>
         <v>0.61299999999999999</v>
       </c>
-      <c r="I18" s="24">
+      <c r="I18" s="23">
         <f t="shared" si="4"/>
         <v>1075</v>
       </c>
@@ -1301,23 +1298,23 @@
         <f t="shared" si="5"/>
         <v>9.6009879999900001</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="24">
         <f t="shared" si="2"/>
         <v>0.27280314772862763</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="24">
         <f t="shared" si="2"/>
         <v>3.3265768451174432E-2</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="24">
         <f t="shared" si="2"/>
         <v>0.52462143793966853</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="24">
         <f t="shared" si="2"/>
         <v>0.16930964588052938</v>
       </c>
-      <c r="O18" s="25">
+      <c r="O18" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1331,15 +1328,15 @@
         <f>LowerBasinCuts!B12</f>
         <v>10.857008</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="25">
         <f>LowerBasinCuts!I12/1000</f>
         <v>0.192</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="25">
         <f>LowerBasinCuts!J12/1000</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="25">
         <f>LowerBasinCuts!K12/1000</f>
         <v>0</v>
       </c>
@@ -1347,11 +1344,11 @@
         <f>LowerBasinCuts!O12</f>
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="25">
         <f t="shared" si="6"/>
         <v>0.24100000000000002</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="23">
         <f t="shared" si="4"/>
         <v>1090</v>
       </c>
@@ -1359,23 +1356,23 @@
         <f t="shared" si="5"/>
         <v>10.857008</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="24">
         <f t="shared" si="2"/>
         <v>0.29775088480420137</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="24">
         <f t="shared" si="2"/>
         <v>3.3337138942801686E-2</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="24">
         <f t="shared" si="2"/>
         <v>0.50234044982303916</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="24">
         <f t="shared" si="2"/>
         <v>0.16657152642995776</v>
       </c>
-      <c r="O19" s="25">
+      <c r="O19" s="24">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1526,7 +1523,7 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1572,25 +1569,25 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="M3" s="29" t="s">
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="M3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:16" s="4" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">

</xml_diff>